<commit_message>
Fully working  extraction in fixed length blocks
</commit_message>
<xml_diff>
--- a/weekly_programs.xlsx
+++ b/weekly_programs.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,32 +441,32 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>8-14 DE ENERO</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>15-21 DE ENERO</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>22-28 DE ENERO</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>5-11 DE FEBRERO</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
           <t>12-18 DE FEBRERO</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>15-21 DE ENERO</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>19-25 DE FEBRERO</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>22-28 DE ENERO</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>5-11 DE FEBRERO</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>8-14 DE ENERO</t>
         </is>
       </c>
     </row>
@@ -478,69 +478,69 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
+          <t>JOB 34,35</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>JOB 36,37</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>JOB 38,39</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>SALMOS 1-4</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
           <t>SALMOS 5-7</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>JOB 36,37</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
+      <c r="G2" t="inlineStr">
         <is>
           <t>SALMOS 8-10</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>JOB 38,39</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>SALMOS 1-4</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>JOB 34,35</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Canción 102y oración | Palabras de introducción(1 min.)</t>
+          <t>Canción 102</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Canción 118y oración | Palabras de introducción(1 min.)</t>
+          <t>Canción 30</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Canción 147y oración | Palabras de introducción(1 min.)</t>
+          <t>Canción 147</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Canción 2y oración | Palabras de introducción(1 min.)</t>
+          <t>Canción 11</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Canción 11y oración | Palabras de introducción(1 min.)</t>
+          <t>Canción 150</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Canción 150y oración | Palabras de introducción(1 min.)</t>
+          <t>Canción 118</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Canción 30y oración | Palabras de introducción(1 min.)</t>
+          <t>Canción 2</t>
         </is>
       </c>
     </row>
@@ -589,32 +589,32 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
+          <t>1. ¿Le parece que la vida es injusta?</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>1. Por qué podemos confiar en la promesa de la vida eterna</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>1. ¿Dedica tiempo a observar la creación?</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>1. Póngase de parte del Reino de Dios</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
           <t>1. Sea leal a Jehová sin importar lo que hagan los demás</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>1. Por qué podemos confiar en la promesa de la vida eterna</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
+      <c r="G5" t="inlineStr">
         <is>
           <t>1. “Te alabaré, oh, Jehová”</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>1. ¿Dedica tiempo a observar la creación?</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>1. Póngase de parte del Reino de Dios</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>1. ¿Le parece que la vida es injusta?</t>
         </is>
       </c>
     </row>
@@ -752,12 +752,12 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
+          <t>4. Naturalidad: Lo que hizo Felipe</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
           <t>4. Empiece conversaciones</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>4. Naturalidad: Lo que hizo Felipe</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
@@ -789,98 +789,66 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
+          <t>5. Naturalidad: Imite a Felipe</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>5. Empiece conversaciones</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
           <t>5. Haga revisitas</t>
         </is>
       </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>5. Naturalidad: Imite a Felipe</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>5. Empiece conversaciones</t>
-        </is>
-      </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>NUESTRA VIDA CRISTIANA</t>
-        </is>
-      </c>
+      <c r="A11" t="inlineStr"/>
       <c r="B11" t="inlineStr">
         <is>
+          <t>6. Haga discípulos</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>6. Explique sus creencias</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>6. Discurso</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr">
+        <is>
           <t>6. Haga revisitas</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>6. Explique sus creencias</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
+      <c r="G11" t="inlineStr">
         <is>
           <t>6. Discurso</t>
         </is>
       </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>6. Discurso</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>NUESTRA VIDA CRISTIANA</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>6. Haga discípulos</t>
-        </is>
-      </c>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Canción 116</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
+      <c r="A12" t="inlineStr"/>
+      <c r="B12" t="inlineStr"/>
+      <c r="C12" t="inlineStr"/>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="inlineStr">
         <is>
           <t>7. Explique sus creencias</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>NUESTRA VIDA CRISTIANA</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>NUESTRA VIDA CRISTIANA</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>NUESTRA VIDA CRISTIANA</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>Canción 32</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>NUESTRA VIDA CRISTIANA</t>
-        </is>
-      </c>
+      <c r="G12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>6. Necesidades de la congregación</t>
+          <t>NUESTRA VIDA CRISTIANA</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -890,101 +858,188 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Canción 49</t>
+          <t>NUESTRA VIDA CRISTIANA</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Canción 10</t>
+          <t>NUESTRA VIDA CRISTIANA</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Canción 111</t>
+          <t>NUESTRA VIDA CRISTIANA</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>6. Necesidades de la congregación</t>
+          <t>NUESTRA VIDA CRISTIANA</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>Canción 58</t>
+          <t>NUESTRA VIDA CRISTIANA</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>7. Estudio bíblico de la congregación</t>
+          <t>Canción 116</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
+          <t>Canción 58</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Canción 49</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Canción 111</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Canción 32</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
           <t>Canción 99</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>7. Esté preparado por si necesita tratamiento médico o una intervención quirúrgica</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>7. Cómo predicar informalmente de forma natural</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>7. Meditar en la creación nos ayuda a no perder de vista el cuadro completo</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>7. Estudio bíblico de la congregación</t>
-        </is>
-      </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>7. ¿“Predica la palabra” informalmente con entusiasmo?</t>
+          <t>Canción 10</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Palabras de conclusión(3 mins.)|Canción 54y oración</t>
+          <t>6. Necesidades de la congregación</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
+          <t>7. ¿“Predica la palabra” informalmente con entusiasmo?</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>7. Esté preparado por si necesita tratamiento médico o una intervención quirúrgica</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>7. Meditar en la creación nos ayuda a no perder de vista el cuadro completo</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>6. Necesidades de la congregación</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
           <t>8. Informe de servicio anual</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr">
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>7. Cómo predicar informalmente de forma natural</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>7. Estudio bíblico de la congregación</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
         <is>
           <t>8. Estudio bíblico de la congregación</t>
         </is>
       </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>Las siguientes ideas le servirán para comenzar conversaciones:</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
+      <c r="C16" t="inlineStr">
         <is>
           <t>8. Estudio bíblico de la congregación</t>
         </is>
       </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>Palabras de conclusión(3 mins.)|Canción 61y oración</t>
-        </is>
-      </c>
-      <c r="G15" t="inlineStr">
+      <c r="D16" t="inlineStr">
         <is>
           <t>8. Estudio bíblico de la congregación</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>7. Estudio bíblico de la congregación</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>9. Estudio bíblico de la congregación</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>8. Necesidades de la congregación</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Canción 54</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Canción 138</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Canción 67</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Canción 54</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Canción 61</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Canción 83</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>9. Estudio bíblico de la congregación</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr"/>
+      <c r="B18" t="inlineStr"/>
+      <c r="C18" t="inlineStr"/>
+      <c r="D18" t="inlineStr"/>
+      <c r="E18" t="inlineStr"/>
+      <c r="F18" t="inlineStr"/>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>Canción 65</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
New meeting day format in the xlsx
By default, now it exports the meeting day (Tuesday by default) instead of the week range
</commit_message>
<xml_diff>
--- a/weekly_programs.xlsx
+++ b/weekly_programs.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,47 +436,47 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>1-7 DE ENERO</t>
+          <t>02/01/2024</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>8-14 DE ENERO</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>15-21 DE ENERO</t>
+          <t>16/01/2024</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>22-28 DE ENERO</t>
+          <t>23/01/2024</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>29 DE ENERO A 4 DE FEBRERO</t>
+          <t>30/01/2024</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>5-11 DE FEBRERO</t>
+          <t>06/02/2024</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>12-18 DE FEBRERO</t>
+          <t>13/02/2024</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>19-25 DE FEBRERO</t>
+          <t>20/02/2024</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>26 DE FEBRERO A 3 DE MARZO</t>
+          <t>27/02/2024</t>
         </is>
       </c>
     </row>
@@ -530,47 +530,47 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Canción 102</t>
+          <t>Canción 102y oración | Palabras de introducción(1 min.)</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Canción 30</t>
+          <t>Canción 30y oración | Palabras de introducción(1 min.)</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Canción 147</t>
+          <t>Canción 147y oración | Palabras de introducción(1 min.)</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Canción 11</t>
+          <t>Canción 11y oración | Palabras de introducción(1 min.)</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Canción 124</t>
+          <t>Canción 124y oración | Palabras de introducción(1 min.)</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Canción 150</t>
+          <t>Canción 150y oración | Palabras de introducción(1 min.)</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Canción 118</t>
+          <t>Canción 118y oración | Palabras de introducción(1 min.)</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Canción 2</t>
+          <t>Canción 2y oración | Palabras de introducción(1 min.)</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>Canción 139</t>
+          <t>Canción 139y oración | Palabras de introducción(1 min.)</t>
         </is>
       </c>
     </row>
@@ -904,7 +904,11 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr"/>
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>NUESTRA VIDA CRISTIANA</t>
+        </is>
+      </c>
       <c r="B11" t="inlineStr">
         <is>
           <t>6. Haga discípulos</t>
@@ -925,7 +929,11 @@
           <t>6. Discurso</t>
         </is>
       </c>
-      <c r="F11" t="inlineStr"/>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>NUESTRA VIDA CRISTIANA</t>
+        </is>
+      </c>
       <c r="G11" t="inlineStr">
         <is>
           <t>6. Haga revisitas</t>
@@ -943,18 +951,46 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr"/>
-      <c r="B12" t="inlineStr"/>
-      <c r="C12" t="inlineStr"/>
-      <c r="D12" t="inlineStr"/>
-      <c r="E12" t="inlineStr"/>
-      <c r="F12" t="inlineStr"/>
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Canción 116</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>NUESTRA VIDA CRISTIANA</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>NUESTRA VIDA CRISTIANA</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>NUESTRA VIDA CRISTIANA</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>NUESTRA VIDA CRISTIANA</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Canción 32</t>
+        </is>
+      </c>
       <c r="G12" t="inlineStr">
         <is>
           <t>7. Explique sus creencias</t>
         </is>
       </c>
-      <c r="H12" t="inlineStr"/>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>NUESTRA VIDA CRISTIANA</t>
+        </is>
+      </c>
       <c r="I12" t="inlineStr">
         <is>
           <t>7. Haga discípulos</t>
@@ -964,42 +1000,42 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
+          <t>6. Necesidades de la congregación</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Canción 58</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Canción 49</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Canción 111</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Canción 108</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>6. Necesidades de la congregación</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
           <t>NUESTRA VIDA CRISTIANA</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>NUESTRA VIDA CRISTIANA</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>NUESTRA VIDA CRISTIANA</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>NUESTRA VIDA CRISTIANA</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>NUESTRA VIDA CRISTIANA</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>NUESTRA VIDA CRISTIANA</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>NUESTRA VIDA CRISTIANA</t>
-        </is>
-      </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>NUESTRA VIDA CRISTIANA</t>
+          <t>Canción 10</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
@@ -1011,32 +1047,32 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Canción 116</t>
+          <t>7. Estudio bíblico de la congregación</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Canción 58</t>
+          <t>7. ¿“Predica la palabra” informalmente con entusiasmo?</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Canción 49</t>
+          <t>7. Esté preparado por si necesita tratamiento médico o una intervención quirúrgica</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Canción 111</t>
+          <t>7. Meditar en la creación nos ayuda a no perder de vista el cuadro completo</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Canción 108</t>
+          <t>7. Ayude a los demás a sentir el amor de Jehová</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Canción 32</t>
+          <t>7. Estudio bíblico de la congregación</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
@@ -1046,7 +1082,7 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>Canción 10</t>
+          <t>7. Cómo predicar informalmente de forma natural</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
@@ -1058,32 +1094,32 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>6. Necesidades de la congregación</t>
+          <t>Palabras de conclusión(3 mins.)|Canción 54y oración</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>7. ¿“Predica la palabra” informalmente con entusiasmo?</t>
+          <t>8. Estudio bíblico de la congregación</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>7. Esté preparado por si necesita tratamiento médico o una intervención quirúrgica</t>
+          <t>8. Estudio bíblico de la congregación</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>7. Meditar en la creación nos ayuda a no perder de vista el cuadro completo</t>
+          <t>8. Estudio bíblico de la congregación</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>7. Ayude a los demás a sentir el amor de Jehová</t>
+          <t>¿Cómo podemos ayudar a nuestros hermanos a creer que Jehová los ama?</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>6. Necesidades de la congregación</t>
+          <t>Palabras de conclusión(3 mins.)|Canción 61y oración</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
@@ -1093,125 +1129,12 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>7. Cómo predicar informalmente de forma natural</t>
+          <t>Las siguientes ideas le servirán para comenzar conversaciones:</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
           <t>8. “La sabiduría es mejor que las armas de guerra”</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>7. Estudio bíblico de la congregación</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>8. Estudio bíblico de la congregación</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>8. Estudio bíblico de la congregación</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>8. Estudio bíblico de la congregación</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>8. Estudio bíblico de la congregación</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>7. Estudio bíblico de la congregación</t>
-        </is>
-      </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>9. Estudio bíblico de la congregación</t>
-        </is>
-      </c>
-      <c r="H16" t="inlineStr">
-        <is>
-          <t>8. Necesidades de la congregación</t>
-        </is>
-      </c>
-      <c r="I16" t="inlineStr">
-        <is>
-          <t>9. El sábado 2 de marzo comienza la campaña de la Conmemoración</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr"/>
-      <c r="B17" t="inlineStr"/>
-      <c r="C17" t="inlineStr"/>
-      <c r="D17" t="inlineStr"/>
-      <c r="E17" t="inlineStr"/>
-      <c r="F17" t="inlineStr"/>
-      <c r="G17" t="inlineStr"/>
-      <c r="H17" t="inlineStr">
-        <is>
-          <t>9. Estudio bíblico de la congregación</t>
-        </is>
-      </c>
-      <c r="I17" t="inlineStr">
-        <is>
-          <t>10. Estudio bíblico de la congregación</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>Canción 54</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>Canción 138</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>Canción 67</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>Canción 54</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>Canción 126</t>
-        </is>
-      </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>Canción 61</t>
-        </is>
-      </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>Canción 83</t>
-        </is>
-      </c>
-      <c r="H18" t="inlineStr">
-        <is>
-          <t>Canción 65</t>
-        </is>
-      </c>
-      <c r="I18" t="inlineStr">
-        <is>
-          <t>Canción 40</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Format and extraction fixed. Weekly programs are always sorted
</commit_message>
<xml_diff>
--- a/weekly_programs.xlsx
+++ b/weekly_programs.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,141 +436,141 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>02/01/2024</t>
+          <t>05/03/2024</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>09/01/2024</t>
+          <t>12/03/2024</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>16/01/2024</t>
+          <t>19/03/2024</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>23/01/2024</t>
+          <t>26/03/2024</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>30/01/2024</t>
+          <t>02/04/2024</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>06/02/2024</t>
+          <t>09/04/2024</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>13/02/2024</t>
+          <t>16/04/2024</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>20/02/2024</t>
+          <t>23/04/2024</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>27/02/2024</t>
+          <t>30/04/2024</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>JOB 32,33</t>
+          <t>SALMOS 16,17</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>JOB 34,35</t>
+          <t>SALMO 18</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>JOB 36,37</t>
+          <t>SALMOS 19-21</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>JOB 38,39</t>
+          <t>SALMO 22</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>JOB 40-42</t>
+          <t>SALMOS 23-25</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>SALMOS 1-4</t>
+          <t>SALMOS 26-28</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>SALMOS 5-7</t>
+          <t>SALMOS 29-31</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>SALMOS 8-10</t>
+          <t>SALMOS 32,33</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>SALMOS 11-15</t>
+          <t>SALMOS 34,35</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Canción 102y oración | Palabras de introducción(1 min.)</t>
+          <t>Canción 111y oración | Palabras de introducción(1 min.)</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Canción 30y oración | Palabras de introducción(1 min.)</t>
+          <t>Canción 148y oración | Palabras de introducción(1 min.)</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Canción 147y oración | Palabras de introducción(1 min.)</t>
+          <t>Canción 6y oración | Palabras de introducción(1 min.)</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Canción 11y oración | Palabras de introducción(1 min.)</t>
+          <t>Canción 19y oración | Palabras de introducción(1 min.)</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Canción 124y oración | Palabras de introducción(1 min.)</t>
+          <t>Canción 4y oración | Palabras de introducción(1 min.)</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Canción 150y oración | Palabras de introducción(1 min.)</t>
+          <t>Canción 34y oración | Palabras de introducción(1 min.)</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Canción 118y oración | Palabras de introducción(1 min.)</t>
+          <t>Canción 108y oración | Palabras de introducción(1 min.)</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Canción 2y oración | Palabras de introducción(1 min.)</t>
+          <t>Canción 103y oración | Palabras de introducción(1 min.)</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>Canción 139y oración | Palabras de introducción(1 min.)</t>
+          <t>Canción 10y oración | Palabras de introducción(1 min.)</t>
         </is>
       </c>
     </row>
@@ -624,47 +624,47 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>1. Usted puede ayudar a quienes están angustiados</t>
+          <t>1. “Jehová, mi fuente de todo lo bueno”</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>1. ¿Le parece que la vida es injusta?</t>
+          <t>1. “Jehová es [...] mi libertador”</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>1. Por qué podemos confiar en la promesa de la vida eterna</t>
+          <t>1. “Los cielos declaran la gloria de Dios”</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>1. ¿Dedica tiempo a observar la creación?</t>
+          <t>1. Se profetizaron detalles de la muerte de Jesús</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>1. ¿Qué nos enseña la experiencia de Job?</t>
+          <t>1. “Jehová es mi Pastor”</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>1. Póngase de parte del Reino de Dios</t>
+          <t>1. Qué ayudaba a David a vivir con integridad</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>1. Sea leal a Jehová sin importar lo que hagan los demás</t>
+          <t>1. La disciplina es una muestra del amor de Dios</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>1. “Te alabaré, oh, Jehová”</t>
+          <t>1. ¿Por qué deben confesarse los pecados graves?</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>1. Imagínese en un nuevo mundo lleno de paz</t>
+          <t>1. “Alabaré a Jehová en todo momento”</t>
         </is>
       </c>
     </row>
@@ -812,34 +812,34 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>4. Interés sincero:Lo que hizo Jesús</t>
+          <t>4. Empiece conversaciones</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
+          <t>4. Bondad: Lo que hizo Jesús</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
           <t>4. Empiece conversaciones</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="D9" t="inlineStr">
         <is>
           <t>4. Empiece conversaciones</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
+      <c r="E9" t="inlineStr">
         <is>
           <t>4. Empiece conversaciones</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr">
+      <c r="F9" t="inlineStr">
         <is>
           <t>4. Empiece conversaciones</t>
         </is>
       </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>4. Naturalidad: Lo que hizo Felipe</t>
-        </is>
-      </c>
       <c r="G9" t="inlineStr">
         <is>
           <t>4. Empiece conversaciones</t>
@@ -847,7 +847,7 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>4. Empiece conversaciones</t>
+          <t>4. Humildad: Lo que hizo Pablo</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
@@ -859,32 +859,32 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>5. Interés sincero:Imite a Jesús</t>
+          <t>5. Empiece conversaciones</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
+          <t>5. Bondad: Imite a Jesús</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
           <t>5. Empiece conversaciones</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
+      <c r="D10" t="inlineStr">
         <is>
           <t>5. Haga revisitas</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
+      <c r="E10" t="inlineStr">
         <is>
           <t>5. Haga revisitas</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>5. Haga discípulos</t>
-        </is>
-      </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>5. Naturalidad: Imite a Felipe</t>
+          <t>5. Haga revisitas</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
@@ -894,138 +894,102 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
+          <t>5. Humildad: Imite a Pablo</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
           <t>5. Haga revisitas</t>
-        </is>
-      </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>5. Empiece conversaciones</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>NUESTRA VIDA CRISTIANA</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
+          <t>6. Empiece conversaciones</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr"/>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>6. Explique sus creencias</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>6. Discurso</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
         <is>
           <t>6. Haga discípulos</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>6. Discurso</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>6. Haga revisitas</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr"/>
+      <c r="I11" t="inlineStr">
         <is>
           <t>6. Explique sus creencias</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>6. Discurso</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>6. Discurso</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>NUESTRA VIDA CRISTIANA</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>6. Haga revisitas</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>6. Discurso</t>
-        </is>
-      </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>6. Empiece conversaciones</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Canción 116</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>NUESTRA VIDA CRISTIANA</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>NUESTRA VIDA CRISTIANA</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>NUESTRA VIDA CRISTIANA</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>NUESTRA VIDA CRISTIANA</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>Canción 32</t>
-        </is>
-      </c>
+          <t>7. Haga discípulos</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr"/>
+      <c r="C12" t="inlineStr"/>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="inlineStr"/>
       <c r="G12" t="inlineStr">
         <is>
-          <t>7. Explique sus creencias</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>NUESTRA VIDA CRISTIANA</t>
-        </is>
-      </c>
-      <c r="I12" t="inlineStr">
-        <is>
           <t>7. Haga discípulos</t>
         </is>
       </c>
+      <c r="H12" t="inlineStr"/>
+      <c r="I12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>6. Necesidades de la congregación</t>
+          <t>NUESTRA VIDA CRISTIANA</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Canción 58</t>
+          <t>NUESTRA VIDA CRISTIANA</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Canción 49</t>
+          <t>NUESTRA VIDA CRISTIANA</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Canción 111</t>
+          <t>NUESTRA VIDA CRISTIANA</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Canción 108</t>
+          <t>NUESTRA VIDA CRISTIANA</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>6. Necesidades de la congregación</t>
+          <t>NUESTRA VIDA CRISTIANA</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
@@ -1035,7 +999,7 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>Canción 10</t>
+          <t>NUESTRA VIDA CRISTIANA</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
@@ -1047,96 +1011,173 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>7. Estudio bíblico de la congregación</t>
+          <t>Canción 20</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>7. ¿“Predica la palabra” informalmente con entusiasmo?</t>
+          <t>Canción 60</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>7. Esté preparado por si necesita tratamiento médico o una intervención quirúrgica</t>
+          <t>Canción 141</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>7. Meditar en la creación nos ayuda a no perder de vista el cuadro completo</t>
+          <t>Canción 95</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>7. Ayude a los demás a sentir el amor de Jehová</t>
+          <t>Canción 54</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>7. Estudio bíblico de la congregación</t>
+          <t>Canción 128</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>Canción 99</t>
+          <t>Canción 45</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>7. Cómo predicar informalmente de forma natural</t>
+          <t>Canción 74</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>Canción 8</t>
+          <t>Canción 59</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Palabras de conclusión(3 mins.)|Canción 54y oración</t>
+          <t>8. ¡Preparémonos para la Conmemoración!</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
+          <t>6. Necesidades de la congregación</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>7.Observar la creación fortalece la fe</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>7. Necesidades de la congregación</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>7. Rechazamos la voz de los extraños</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>7. Adolescentes que son moralmente íntegros</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>8.Por qué tenemos fe en... el amor de Dios</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>6. Necesidades de la congregación</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>7. Tres formas de alabar a Jehová en nuestras reuniones</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>9. Estudio bíblico de la congregación</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>7.Logros de la organizaciónpara el mes de marzo</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
           <t>8. Estudio bíblico de la congregación</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr">
+      <c r="D16" t="inlineStr">
         <is>
           <t>8. Estudio bíblico de la congregación</t>
         </is>
       </c>
-      <c r="D15" t="inlineStr">
+      <c r="E16" t="inlineStr">
         <is>
           <t>8. Estudio bíblico de la congregación</t>
         </is>
       </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>¿Cómo podemos ayudar a nuestros hermanos a creer que Jehová los ama?</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>Palabras de conclusión(3 mins.)|Canción 61y oración</t>
-        </is>
-      </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>8. Informe de servicio anual</t>
-        </is>
-      </c>
-      <c r="H15" t="inlineStr">
-        <is>
-          <t>Las siguientes ideas le servirán para comenzar conversaciones:</t>
-        </is>
-      </c>
-      <c r="I15" t="inlineStr">
-        <is>
-          <t>8. “La sabiduría es mejor que las armas de guerra”</t>
-        </is>
-      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>8. Estudio bíblico de la congregación</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>9.2024|Informe sobre la actividad del Departamento Local de Diseño y Construcción</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>7. Estudio bíblico de la congregación</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>8. Estudio bíblico de la congregación</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr"/>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>8. Estudio bíblico de la congregación</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr"/>
+      <c r="D17" t="inlineStr"/>
+      <c r="E17" t="inlineStr"/>
+      <c r="F17" t="inlineStr"/>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>10. Estudio bíblico de la congregación</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr"/>
+      <c r="I17" t="inlineStr"/>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr"/>
+      <c r="B18" t="inlineStr"/>
+      <c r="C18" t="inlineStr"/>
+      <c r="D18" t="inlineStr"/>
+      <c r="E18" t="inlineStr"/>
+      <c r="F18" t="inlineStr"/>
+      <c r="G18" t="inlineStr"/>
+      <c r="H18" t="inlineStr"/>
+      <c r="I18" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Canción inicial formato solucionado
</commit_message>
<xml_diff>
--- a/weekly_programs.xlsx
+++ b/weekly_programs.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,141 +436,126 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>05/03/2024</t>
+          <t>07/01/2025</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>12/03/2024</t>
+          <t>14/01/2025</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>19/03/2024</t>
+          <t>21/01/2025</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>26/03/2024</t>
+          <t>28/01/2025</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>02/04/2024</t>
+          <t>04/02/2025</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>09/04/2024</t>
+          <t>11/02/2025</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>16/04/2024</t>
+          <t>18/02/2025</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>23/04/2024</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>30/04/2024</t>
+          <t>25/02/2025</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>SALMOS 16,17</t>
+          <t>SALMOS 127-134</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>SALMO 18</t>
+          <t>SALMOS 135-137</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>SALMOS 19-21</t>
+          <t>SALMOS 138,139</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>SALMO 22</t>
+          <t>SALMOS 140-143</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>SALMOS 23-25</t>
+          <t>SALMOS 144-146</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>SALMOS 26-28</t>
+          <t>SALMOS 147-150</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>SALMOS 29-31</t>
+          <t>PROVERBIOS 1</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>SALMOS 32,33</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>SALMOS 34,35</t>
+          <t>PROVERBIOS 2</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Canción 111y oración | Palabras de introducción(1 min.)</t>
+          <t>Canción 134</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Canción 148y oración | Palabras de introducción(1 min.)</t>
+          <t>Canción 2</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Canción 6y oración | Palabras de introducción(1 min.)</t>
+          <t>Canción 93</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Canción 19y oración | Palabras de introducción(1 min.)</t>
+          <t>Canción 44</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Canción 4y oración | Palabras de introducción(1 min.)</t>
+          <t>Canción 145</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Canción 34y oración | Palabras de introducción(1 min.)</t>
+          <t>Canción 12</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Canción 108y oración | Palabras de introducción(1 min.)</t>
+          <t>Canción 88</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Canción 103y oración | Palabras de introducción(1 min.)</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>Canción 10y oración | Palabras de introducción(1 min.)</t>
+          <t>Canción 35</t>
         </is>
       </c>
     </row>
@@ -615,56 +600,46 @@
           <t>TESOROS DE LA BIBLIA</t>
         </is>
       </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>TESOROS DE LA BIBLIA</t>
-        </is>
-      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>1. “Jehová, mi fuente de todo lo bueno”</t>
+          <t>1. Padres, sigan cuidando la herencia que Jehová les dio</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>1. “Jehová es [...] mi libertador”</t>
+          <t>1. “Nuestro Señor es más grande que todos los demás dioses”</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>1. “Los cielos declaran la gloria de Dios”</t>
+          <t>1. ¡Que los nervios no lo frenen!</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>1. Se profetizaron detalles de la muerte de Jesús</t>
+          <t>1. ¿Qué hará después de orar?</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>1. “Jehová es mi Pastor”</t>
+          <t>1. “¡Feliz el pueblo que tiene por Dios a Jehová!”</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>1. Qué ayudaba a David a vivir con integridad</t>
+          <t>1. Tenemos muchas razones para alabar a Jah</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>1. La disciplina es una muestra del amor de Dios</t>
+          <t>1. Joven, ¿a quién escucharás?</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>1. ¿Por qué deben confesarse los pecados graves?</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>1. “Alabaré a Jehová en todo momento”</t>
+          <t>1. Por qué estudiar con ganas</t>
         </is>
       </c>
     </row>
@@ -709,11 +684,6 @@
           <t>2. Busquemos perlas escondidas</t>
         </is>
       </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>2. Busquemos perlas escondidas</t>
-        </is>
-      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -756,11 +726,6 @@
           <t>3. Lectura de la Biblia</t>
         </is>
       </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>3. Lectura de la Biblia</t>
-        </is>
-      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -803,11 +768,6 @@
           <t>SEAMOS MEJORES MAESTROS</t>
         </is>
       </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>SEAMOS MEJORES MAESTROS</t>
-        </is>
-      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -817,7 +777,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>4. Bondad: Lo que hizo Jesús</t>
+          <t>4. Empiece conversaciones</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -846,11 +806,6 @@
         </is>
       </c>
       <c r="H9" t="inlineStr">
-        <is>
-          <t>4. Humildad: Lo que hizo Pablo</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr">
         <is>
           <t>4. Empiece conversaciones</t>
         </is>
@@ -864,40 +819,35 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>5. Bondad: Imite a Jesús</t>
+          <t>5. Haga revisitas</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
+          <t>5. Haga discípulos</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>5. Haga revisitas</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>5. Haga revisitas</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
           <t>5. Empiece conversaciones</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>5. Haga revisitas</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>5. Haga revisitas</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>5. Haga revisitas</t>
-        </is>
-      </c>
       <c r="G10" t="inlineStr">
         <is>
           <t>5. Empiece conversaciones</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
-        <is>
-          <t>5. Humildad: Imite a Pablo</t>
-        </is>
-      </c>
-      <c r="I10" t="inlineStr">
         <is>
           <t>5. Haga revisitas</t>
         </is>
@@ -906,25 +856,29 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>6. Empiece conversaciones</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr"/>
+          <t>6. Haga discípulos</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>6. Explique sus creencias</t>
+        </is>
+      </c>
       <c r="C11" t="inlineStr">
         <is>
+          <t>6. Discurso</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
           <t>6. Explique sus creencias</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
+      <c r="E11" t="inlineStr">
         <is>
           <t>6. Discurso</t>
         </is>
       </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>6. Haga discípulos</t>
-        </is>
-      </c>
       <c r="F11" t="inlineStr">
         <is>
           <t>6. Discurso</t>
@@ -935,19 +889,14 @@
           <t>6. Haga revisitas</t>
         </is>
       </c>
-      <c r="H11" t="inlineStr"/>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>6. Explique sus creencias</t>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>6. Discurso</t>
         </is>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>7. Haga discípulos</t>
-        </is>
-      </c>
+      <c r="A12" t="inlineStr"/>
       <c r="B12" t="inlineStr"/>
       <c r="C12" t="inlineStr"/>
       <c r="D12" t="inlineStr"/>
@@ -959,7 +908,6 @@
         </is>
       </c>
       <c r="H12" t="inlineStr"/>
-      <c r="I12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1002,182 +950,200 @@
           <t>NUESTRA VIDA CRISTIANA</t>
         </is>
       </c>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>NUESTRA VIDA CRISTIANA</t>
-        </is>
-      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Canción 20</t>
+          <t>Canción 13</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Canción 60</t>
+          <t>Canción 10</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
+          <t>Canción 59</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
           <t>Canción 141</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>Canción 95</t>
-        </is>
-      </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Canción 54</t>
+          <t>Canción 59</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Canción 128</t>
+          <t>Canción 159</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>Canción 45</t>
+          <t>Canción 89</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>Canción 74</t>
-        </is>
-      </c>
-      <c r="I14" t="inlineStr">
-        <is>
-          <t>Canción 59</t>
+          <t>Canción 96</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>8. ¡Preparémonos para la Conmemoración!</t>
+          <t>7. Padres, ¿están usando esta herramienta tan potente?</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>6. Necesidades de la congregación</t>
+          <t>7. Necesidades de la congregación</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>7.Observar la creación fortalece la fe</t>
+          <t>7. Aunque sea tímido, puede tener éxito sirviendo a Jehová</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>7. Necesidades de la congregación</t>
+          <t>7. Esté preparado por si necesita atención médica o una intervención quirúrgica</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>7. Rechazamos la voz de los extraños</t>
+          <t>7. Jehová quiere que usted sea feliz</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>7. Adolescentes que son moralmente íntegros</t>
+          <t>7. Informe de servicio anual</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>8.Por qué tenemos fe en... el amor de Dios</t>
+          <t>8. Necesidades de la congregación</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>6. Necesidades de la congregación</t>
-        </is>
-      </c>
-      <c r="I15" t="inlineStr">
-        <is>
-          <t>7. Tres formas de alabar a Jehová en nuestras reuniones</t>
+          <t>7. ¿Eres un cazatesoros?</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
+          <t>Gracias a su ejemplo, sus hijos pueden aprender a...</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>8. Estudio bíblico de la congregación</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>8. Estudio bíblico de la congregación</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>¿ESTÁ PREPARADO?</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>8. Necesidades de la congregación</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>8. Estudio bíblico de la congregación</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
           <t>9. Estudio bíblico de la congregación</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>7.Logros de la organizaciónpara el mes de marzo</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>SUGERENCIA</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
         <is>
           <t>8. Estudio bíblico de la congregación</t>
         </is>
       </c>
-      <c r="D16" t="inlineStr">
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Palabras de conclusión(3 mins.)|Canción 90y oración</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Palabras de conclusión(3 mins.)|Canción 151y oración</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
         <is>
           <t>8. Estudio bíblico de la congregación</t>
         </is>
       </c>
-      <c r="E16" t="inlineStr">
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>9. Estudio bíblico de la congregación</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Palabras de conclusión(3 mins.)|Canción 37y oración</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>Palabras de conclusión(3 mins.)|Canción 80y oración</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
         <is>
           <t>8. Estudio bíblico de la congregación</t>
         </is>
       </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>8. Estudio bíblico de la congregación</t>
-        </is>
-      </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>9.2024|Informe sobre la actividad del Departamento Local de Diseño y Construcción</t>
-        </is>
-      </c>
-      <c r="H16" t="inlineStr">
-        <is>
-          <t>7. Estudio bíblico de la congregación</t>
-        </is>
-      </c>
-      <c r="I16" t="inlineStr">
-        <is>
-          <t>8. Estudio bíblico de la congregación</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr"/>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>8. Estudio bíblico de la congregación</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr"/>
-      <c r="D17" t="inlineStr"/>
-      <c r="E17" t="inlineStr"/>
-      <c r="F17" t="inlineStr"/>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>10. Estudio bíblico de la congregación</t>
-        </is>
-      </c>
-      <c r="H17" t="inlineStr"/>
-      <c r="I17" t="inlineStr"/>
     </row>
     <row r="18">
-      <c r="A18" t="inlineStr"/>
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Palabras de conclusión(3 mins.)|Canción 73y oración</t>
+        </is>
+      </c>
       <c r="B18" t="inlineStr"/>
       <c r="C18" t="inlineStr"/>
-      <c r="D18" t="inlineStr"/>
-      <c r="E18" t="inlineStr"/>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Palabras de conclusión(3 mins.)|Canción 103y oración</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Palabras de conclusión(3 mins.)|Canción 85y oración</t>
+        </is>
+      </c>
       <c r="F18" t="inlineStr"/>
       <c r="G18" t="inlineStr"/>
-      <c r="H18" t="inlineStr"/>
-      <c r="I18" t="inlineStr"/>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>Palabras de conclusión(3 mins.)|Canción 102y oración</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Last Song formatting now fixed
The last song is now properly parsed and placed at the end of NVC
Also, if there is a "weird" week (Like Conmemoración), it is skipped
</commit_message>
<xml_diff>
--- a/weekly_programs.xlsx
+++ b/weekly_programs.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1083,16 +1083,8 @@
           <t>8. Estudio bíblico de la congregación</t>
         </is>
       </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>Palabras de conclusión(3 mins.)|Canción 90y oración</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>Palabras de conclusión(3 mins.)|Canción 151y oración</t>
-        </is>
-      </c>
+      <c r="B17" t="inlineStr"/>
+      <c r="C17" t="inlineStr"/>
       <c r="D17" t="inlineStr">
         <is>
           <t>8. Estudio bíblico de la congregación</t>
@@ -1103,16 +1095,8 @@
           <t>9. Estudio bíblico de la congregación</t>
         </is>
       </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>Palabras de conclusión(3 mins.)|Canción 37y oración</t>
-        </is>
-      </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>Palabras de conclusión(3 mins.)|Canción 80y oración</t>
-        </is>
-      </c>
+      <c r="F17" t="inlineStr"/>
+      <c r="G17" t="inlineStr"/>
       <c r="H17" t="inlineStr">
         <is>
           <t>8. Estudio bíblico de la congregación</t>
@@ -1120,28 +1104,54 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>Palabras de conclusión(3 mins.)|Canción 73y oración</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr"/>
-      <c r="C18" t="inlineStr"/>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>Palabras de conclusión(3 mins.)|Canción 103y oración</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>Palabras de conclusión(3 mins.)|Canción 85y oración</t>
-        </is>
-      </c>
-      <c r="F18" t="inlineStr"/>
-      <c r="G18" t="inlineStr"/>
-      <c r="H18" t="inlineStr">
-        <is>
-          <t>Palabras de conclusión(3 mins.)|Canción 102y oración</t>
+      <c r="A18" t="inlineStr"/>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Canción 90</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Canción 151</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr"/>
+      <c r="E18" t="inlineStr"/>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>Canción 37</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>Canción 80</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr"/>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Canción 73</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr"/>
+      <c r="C19" t="inlineStr"/>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Canción 103</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Canción 85</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr"/>
+      <c r="G19" t="inlineStr"/>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>Canción 102</t>
         </is>
       </c>
     </row>

</xml_diff>